<commit_message>
excel to python code success
</commit_message>
<xml_diff>
--- a/healthcare/healthcarePackage/data.xlsx
+++ b/healthcare/healthcarePackage/data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{32CFB691-F93D-49EA-B420-BE0CDA043419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{3664B7F0-8CDC-4C78-8DDB-A3EC79AB7C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="29070" windowHeight="16500" xr2:uid="{15FF64ED-9A39-45C8-9B4F-47D42B8B8433}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="29100" windowHeight="16500" xr2:uid="{15FF64ED-9A39-45C8-9B4F-47D42B8B8433}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,33 +21,159 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>NAME</t>
   </si>
   <si>
-    <t>AGE</t>
-  </si>
-  <si>
-    <t>Ken</t>
-  </si>
-  <si>
-    <t>Jack</t>
-  </si>
-  <si>
-    <t>Lorraine</t>
-  </si>
-  <si>
-    <t>Cat</t>
-  </si>
-  <si>
-    <t>Kez</t>
-  </si>
-  <si>
-    <t>Bon</t>
+    <t xml:space="preserve">Evalyn  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rose  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freda  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wynona  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tammera  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shantay  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liza  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deetta  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charla  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Milda  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tonette  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suzanna  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elsy  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Winifred  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phylis  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pearl  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maddie  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnolia  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christi  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yolonda  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lavera  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arnetta  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mazie  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remedios  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kimberli  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Page  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olen  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dagmar  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carolin  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leonel  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grazyna  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alda  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cliff  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mauro  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anglea  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Devorah  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patience  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maryland  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shasta  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sueann  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luana  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brynn  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jenni  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eula  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linh  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cara  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elton  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lenna  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lovetta  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merissa  </t>
   </si>
 </sst>
 </file>
@@ -83,8 +209,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,91 +528,271 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCCE51DE-A78C-411E-9C77-FF8933E1607F}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="49" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7">
-        <v>24</v>
-      </c>
-    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
all functions are working
</commit_message>
<xml_diff>
--- a/healthcare/healthcarePackage/data.xlsx
+++ b/healthcare/healthcarePackage/data.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{1EBC25B9-2999-4FD7-B078-538C8FF043B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{E482784F-2255-4719-8BCD-D51FDC91D76A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="29100" windowHeight="16500" activeTab="1" xr2:uid="{15FF64ED-9A39-45C8-9B4F-47D42B8B8433}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="29130" windowHeight="16500" activeTab="1" xr2:uid="{15FF64ED-9A39-45C8-9B4F-47D42B8B8433}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="wound_assessment" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:J19"/>
+  <oleSize ref="A1:F22"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -956,8 +956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{238E7811-4CE6-4971-A252-225B27044111}">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>